<commit_message>
grade added to teacher class
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init.xlsx
+++ b/src/main/resources/xlsx/init.xlsx
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +481,7 @@
     <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -491,8 +491,11 @@
       <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -502,8 +505,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -513,8 +519,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -524,8 +533,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -535,8 +547,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -546,8 +561,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -557,8 +575,11 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -568,8 +589,11 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -579,8 +603,11 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -590,8 +617,11 @@
       <c r="C11">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -601,8 +631,11 @@
       <c r="C13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -612,8 +645,11 @@
       <c r="C14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -623,8 +659,11 @@
       <c r="C15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -634,8 +673,11 @@
       <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -645,8 +687,11 @@
       <c r="C17">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -656,8 +701,11 @@
       <c r="C19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -667,8 +715,11 @@
       <c r="C20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -678,8 +729,11 @@
       <c r="C21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -689,8 +743,11 @@
       <c r="C22">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -700,8 +757,11 @@
       <c r="C24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -711,8 +771,11 @@
       <c r="C25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -722,8 +785,11 @@
       <c r="C26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -732,6 +798,9 @@
       </c>
       <c r="C27">
         <v>5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can create timetable for unique grade
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init.xlsx
+++ b/src/main/resources/xlsx/init.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Russian1</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>1,3</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>№ lesson</t>
+  </si>
+  <si>
+    <t>Day of the week</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
@@ -153,9 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -470,336 +483,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="D24">
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added equalsIgnoreCase() for grades
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/init.xlsx
+++ b/src/main/resources/xlsx/init.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Russian1</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>2a</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,8 +526,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,8 +540,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>2</v>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,8 +554,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,8 +568,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,8 +582,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>2</v>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,8 +596,8 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,8 +610,8 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,8 +624,8 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,8 +638,8 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,8 +652,8 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,8 +666,8 @@
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,8 +680,8 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,8 +694,8 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,8 +708,8 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,8 +722,8 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="2">
-        <v>1</v>
+      <c r="D18" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,8 +736,8 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="2">
-        <v>1</v>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,8 +750,8 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21" s="2">
-        <v>1</v>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,8 +764,8 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22" s="2">
-        <v>1</v>
+      <c r="D22" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,8 +778,8 @@
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23" s="2">
-        <v>1</v>
+      <c r="D23" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,8 +792,8 @@
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25" s="2">
-        <v>1</v>
+      <c r="D25" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,8 +806,8 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="2">
-        <v>1</v>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,8 +820,8 @@
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
+      <c r="D27" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,8 +834,8 @@
       <c r="C28">
         <v>5</v>
       </c>
-      <c r="D28" s="2">
-        <v>1</v>
+      <c r="D28" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>